<commit_message>
worked on code to pyhtonically update the db via sqlite queries
</commit_message>
<xml_diff>
--- a/prep_and_checklists/Stefanie Gal Bridal Shower  /PREPLIST_Stefanie Gal Bridal Shower  _08-15-2025_0.xlsx
+++ b/prep_and_checklists/Stefanie Gal Bridal Shower  /PREPLIST_Stefanie Gal Bridal Shower  _08-15-2025_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcuvin/purveyor_project/prep_and_checklists/Stefanie Gal Bridal Shower  /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81E6C0F-14E6-0B4A-B6C8-89C6940A4A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A873700C-2CCC-C144-A860-882DEECCB1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prep_sheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="120">
   <si>
     <t xml:space="preserve">Stefanie Gal Bridal Shower  , Guests: 60   , 7:00 PM - 10:00 PM   ,Thursday, September 4, 2025  </t>
   </si>
@@ -131,9 +131,6 @@
     <t>clean / grill fish</t>
   </si>
   <si>
-    <t>green olive gremolata</t>
-  </si>
-  <si>
     <t>grilled lemon halves</t>
   </si>
   <si>
@@ -323,9 +320,6 @@
     <t>6 whole lemons</t>
   </si>
   <si>
-    <t>2 cases</t>
-  </si>
-  <si>
     <t>3 cases</t>
   </si>
   <si>
@@ -381,6 +375,12 @@
   </si>
   <si>
     <t>1/2 case</t>
+  </si>
+  <si>
+    <t>lemon caper condiment</t>
+  </si>
+  <si>
+    <t>3 cups</t>
   </si>
 </sst>
 </file>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -877,11 +877,11 @@
     </row>
     <row r="4" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="11"/>
       <c r="D4" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" s="8"/>
     </row>
@@ -904,13 +904,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -918,13 +918,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -932,13 +932,13 @@
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -946,7 +946,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -968,7 +968,7 @@
         <v>24</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -976,13 +976,13 @@
         <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -990,27 +990,27 @@
         <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1018,13 +1018,13 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1032,7 +1032,7 @@
         <v>32</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -1046,7 +1046,7 @@
         <v>34</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1054,15 +1054,15 @@
         <v>35</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>7</v>
@@ -1073,16 +1073,16 @@
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1090,65 +1090,65 @@
         <v>16</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>8</v>
@@ -1162,12 +1162,12 @@
         <v>13</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
@@ -1176,26 +1176,26 @@
         <v>17</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>5</v>
@@ -1203,29 +1203,29 @@
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="D32" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>5</v>
@@ -1233,13 +1233,13 @@
     </row>
     <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>5</v>
@@ -1247,35 +1247,33 @@
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>5</v>
@@ -1283,18 +1281,18 @@
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +1317,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
@@ -1329,175 +1327,175 @@
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>